<commit_message>
fix nhap diem :(
</commit_message>
<xml_diff>
--- a/TemplateNhapDiemDotThi.xlsx
+++ b/TemplateNhapDiemDotThi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\CaoThangAngular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieu1\Desktop\CaoThangAngular\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>hoten</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>36483</t>
   </si>
 </sst>
 </file>
@@ -431,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,8 +505,8 @@
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1">
-        <v>36483</v>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -517,17 +523,17 @@
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1">
-        <v>10</v>
-      </c>
-      <c r="J2" s="1">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1">
-        <v>10</v>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>